<commit_message>
separated +ve supplies and moved LEDs to board edge
</commit_message>
<xml_diff>
--- a/pcb/R1007_BOM.xlsx
+++ b/pcb/R1007_BOM.xlsx
@@ -212,7 +212,7 @@
     <t>Toshiba Semiconductor and Storage</t>
   </si>
   <si>
-    <t>TLP293-4(GB-TP,E</t>
+    <t>TLP293-4(TP,E</t>
   </si>
 </sst>
 </file>
@@ -311,20 +311,20 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.6632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.37755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.719387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.7959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.1326530612245"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.76530612244898"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.6071428571429"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.3316326530612"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.90816326530612"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.73469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.38775510204082"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.95408163265306"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.15816326530612"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.23469387755102"/>

</xml_diff>